<commit_message>
added examples Scopes_03.._04 upgrade to lfet_230325a_upd is needed up from example Scopes_04
</commit_message>
<xml_diff>
--- a/!Beispiele.Übersicht.xlsx
+++ b/!Beispiele.Übersicht.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LF\Projekte\lfet-help-de_workstuff\test_generation\scopes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LF\Projekte\rulebased.group\lfet-examples-scope-de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839397C7-EBB1-4AB3-812C-5B7A2585C69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A310C01D-8BF7-41E9-BC11-D843902974E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20230325 101231" sheetId="1" r:id="rId1"/>
+    <sheet name="20230325 200847" sheetId="1" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20230325 101231'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20230325 200847'!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Nr</t>
   </si>
@@ -149,13 +149,20 @@
     <t>Scopes_01</t>
   </si>
   <si>
-    <t>Beispiel 01: Einfache ET, keine Regelgruppen, nur einfache Testanweisungen, keine Scopes, keine SIDs</t>
+    <t>Beispiel 01: Einfache ET, keine Regelgruppen, keine Scopes/SIDs</t>
+  </si>
+  <si>
+    <t>In dieser Entscheidungstabellen werden alle verfügbaren Testanweisungen genutzt,
+um deren Positionierung im Testfall zu demonstrieren.
+Die folgenden Testanweisungen werden nur in besonderen Fällen genutzt:
+- Anweisungen für nicht verwendete Aktionen
+- Anweisungen für Regeln</t>
   </si>
   <si>
     <t>lfhl</t>
   </si>
   <si>
-    <t>20230325 1010</t>
+    <t>20230325 1501</t>
   </si>
   <si>
     <t>LF-ET 2.2.1 (230323a)</t>
@@ -164,22 +171,57 @@
     <t>Scopes_02</t>
   </si>
   <si>
-    <t>Beispiel 02: ET mit Regelgruppen, nur einfache Testanweisungen, keine Scopes, keine SIDs</t>
-  </si>
-  <si>
-    <t>Diese Datei wurde erzeugt durch LF-ET 2.2.1 (230323a) und Kommandozeile:</t>
-  </si>
-  <si>
-    <t>-List-ET "D:/LF/Projekte/lfet-help-de_workstuff/test_generation/scopes" -Recursive -FileOut "LFET-List-ET.xlsx" -RootDirectory -OpenDirectoryOut -OpenFileOut</t>
+    <t>Beispiel 02: ET mit Regelgruppen, keine Scopes/SIDs</t>
+  </si>
+  <si>
+    <t>In dieser Entscheidungstabellen werden alle verfügbaren Testanweisungen genutzt,
+um deren Positionierung im Testfall zu demonstrieren.
+Die folgenden Testanweisungen werden nur in besonderen Fällen genutzt:
+- Anweisungen für die Regelgruppen-Bedingung, Regelgruppen-Aktion und deren Werte
+- Anweisungen für nicht verwendete Aktionen
+- Anweisungen für Regeln</t>
+  </si>
+  <si>
+    <t>Scopes_03</t>
+  </si>
+  <si>
+    <t>Beispiel 03: ET mit Regelgruppen, keine Scopes/SIDs, mehrfaches Vorkommen von Anweisungen in Testfällen</t>
+  </si>
+  <si>
+    <t>In den vorherigen Entscheidungstabellen wurden alle verfügbaren Testanweisungen genutzt,
+um deren Positionierung im Testfall zu demonstrieren.
+Diese Entscheidungstabelle wurde bereinigt, die nur in Ausnahmefällen benötigten Testanweisungen wurden entfernt.
+Nicht mehr enthalten sind deswegen:
+- Anweisungen für die Regelgruppen-Bedingung,Regelgruppen-Aktion und deren Werte
+- Anweisungen für nicht verwendete Aktionen
+- Anweisungen für Regeln</t>
+  </si>
+  <si>
+    <t>20230325 1504</t>
+  </si>
+  <si>
+    <t>Scopes_04</t>
+  </si>
+  <si>
+    <t>Beispiel 03: ET mit Regelgruppen, Scopes ohne SIDs</t>
+  </si>
+  <si>
+    <t>20230325 1517</t>
+  </si>
+  <si>
+    <t>Diese Datei wurde erzeugt durch LF-ET 2.2.1 (230325a) und Kommandozeile:</t>
+  </si>
+  <si>
+    <t>-List-ET "D:/LF/Projekte/rulebased.group/lfet-examples-scope-de/" -Recursive -FileOut "!Beispiele.Übersicht.xlsx" -RootDirectory -OpenDirectoryOut -OpenFileOut</t>
   </si>
   <si>
     <t>Aktueller Benutzer: lfhl</t>
   </si>
   <si>
-    <t>Aktuelles Verzeichnis (user.dir): "D:\LF\Development\LFET"</t>
-  </si>
-  <si>
-    <t>Benötigte Zeit: 00:00:00.670 (25.03.2023 10:12:31.145 - 25.03.2023 10:12:31.815)</t>
+    <t>Aktuelles Verzeichnis (user.dir): "C:\Program Files\JetBrains\IntelliJ IDEA Community Edition 2022.1.2\jbr\bin"</t>
+  </si>
+  <si>
+    <t>Benötigte Zeit: 00:00:00.228 (25.03.2023 20:08:47.860 - 25.03.2023 20:08:48.088)</t>
   </si>
 </sst>
 </file>
@@ -601,22 +643,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
+    <col min="6" max="9" width="5.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.5703125" customWidth="1"/>
@@ -625,7 +668,7 @@
     <col min="16" max="16" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5">
         <v>2</v>
@@ -707,13 +750,13 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>16</v>
@@ -730,13 +773,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5">
         <v>3</v>
@@ -751,18 +794,106 @@
         <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="K4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>6</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -773,14 +904,18 @@
     <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;P / &amp;N&amp;L&amp;D &amp;T&amp;R&amp;F [ 20230325 101231 ]</oddHeader>
+    <oddHeader>&amp;C&amp;P / &amp;N&amp;L&amp;D &amp;T&amp;R&amp;F [ 20230325 200847 ]</oddHeader>
   </headerFooter>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -801,12 +936,12 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -816,17 +951,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>